<commit_message>
converted to json for biometric
</commit_message>
<xml_diff>
--- a/ExcelFiles/HRNet.xlsx
+++ b/ExcelFiles/HRNet.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saurabh\Documents\GitHub\ExcelReader\ExcelFiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="5904"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="5910"/>
   </bookViews>
   <sheets>
     <sheet name="report1453261047324" sheetId="1" r:id="rId1"/>
@@ -17,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="47">
   <si>
     <t>Worker: Worker ID</t>
   </si>
@@ -134,12 +139,36 @@
   </si>
   <si>
     <t>Request ID-00000286</t>
+  </si>
+  <si>
+    <t>R100</t>
+  </si>
+  <si>
+    <t>R102</t>
+  </si>
+  <si>
+    <t>R104</t>
+  </si>
+  <si>
+    <t>R125</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R40</t>
+  </si>
+  <si>
+    <t>R84</t>
+  </si>
+  <si>
+    <t>R106</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -944,7 +973,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -952,24 +981,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -995,35 +1024,38 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>1477</v>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G2" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="J2" s="2">
+        <v>1477</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>1477</v>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>8</v>
@@ -1037,45 +1069,51 @@
       <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>13</v>
+      <c r="F3" s="4">
+        <v>42398</v>
       </c>
       <c r="G3" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="J3" s="2">
+        <v>1477</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>1477</v>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G4" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="J4" s="2">
+        <v>1477</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>1482</v>
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>16</v>
@@ -1098,62 +1136,71 @@
       <c r="H5" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="J5" s="2">
+        <v>1482</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="4">
+        <v>42461</v>
+      </c>
+      <c r="F6" s="4">
+        <v>42461</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="2">
         <v>1748</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="2">
-        <v>2</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>238</v>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E7" s="4">
-        <v>42461</v>
+        <v>42522</v>
       </c>
       <c r="F7" s="4">
-        <v>42461</v>
+        <v>42522</v>
       </c>
       <c r="G7" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="J7" s="2">
+        <v>238</v>
+      </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>238</v>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>24</v>
@@ -1176,123 +1223,138 @@
       <c r="H8" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="J8" s="2">
+        <v>238</v>
+      </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="4">
+        <v>42552</v>
+      </c>
+      <c r="F9" s="4">
+        <v>42552</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="2">
         <v>238</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="4">
-        <v>42522</v>
-      </c>
-      <c r="F9" s="4">
-        <v>42522</v>
-      </c>
-      <c r="G9" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>24</v>
-      </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>265</v>
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G10" s="2">
         <v>1</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>28</v>
+        <v>33</v>
+      </c>
+      <c r="J10" s="2">
+        <v>265</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <v>1501</v>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>32</v>
+      <c r="E11" s="4">
+        <v>42583</v>
+      </c>
+      <c r="F11" s="4">
+        <v>42583</v>
       </c>
       <c r="G11" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
+      </c>
+      <c r="J11" s="2">
+        <v>1501</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
-        <v>1307</v>
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="4">
-        <v>42583</v>
-      </c>
-      <c r="F12" s="4">
-        <v>42583</v>
+      <c r="E12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="G12" s="2">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>33</v>
+        <v>20</v>
+      </c>
+      <c r="J12" s="2">
+        <v>1307</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
-        <v>1307</v>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>19</v>
@@ -1304,63 +1366,76 @@
         <v>1</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>33</v>
+        <v>37</v>
+      </c>
+      <c r="J13" s="2">
+        <v>1307</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
-        <v>1307</v>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="4">
-        <v>42552</v>
-      </c>
-      <c r="F14" s="4">
-        <v>42552</v>
+        <v>22</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="G14" s="2">
         <v>1</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
+      </c>
+      <c r="J14" s="2">
+        <v>1307</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
-        <v>1535</v>
+    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="G15" s="2">
         <v>1</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
+      </c>
+      <c r="J15" s="2">
+        <v>1535</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H15"/>
+  <autoFilter ref="A1:H15">
+    <sortState ref="A2:H15">
+      <sortCondition ref="C1:C15"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Done the refactoring using the enums Displayed correct leavetype Hrnet file upgraded to have absencedetails
</commit_message>
<xml_diff>
--- a/ExcelFiles/HRNet.xlsx
+++ b/ExcelFiles/HRNet.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saurabh\Documents\GitHub\ExcelReader\ExcelFiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="5904"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="5910"/>
   </bookViews>
   <sheets>
     <sheet name="report1453261047324" sheetId="1" r:id="rId1"/>
@@ -17,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="47">
   <si>
     <t>Worker: Worker ID</t>
   </si>
@@ -134,12 +139,36 @@
   </si>
   <si>
     <t>Request ID-00000286</t>
+  </si>
+  <si>
+    <t>R100</t>
+  </si>
+  <si>
+    <t>R102</t>
+  </si>
+  <si>
+    <t>R104</t>
+  </si>
+  <si>
+    <t>R125</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R40</t>
+  </si>
+  <si>
+    <t>R84</t>
+  </si>
+  <si>
+    <t>R106</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -944,7 +973,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -952,24 +981,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -995,35 +1024,38 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>1477</v>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G2" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="J2" s="2">
+        <v>1477</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>1477</v>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>8</v>
@@ -1037,45 +1069,51 @@
       <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>13</v>
+      <c r="F3" s="4">
+        <v>42398</v>
       </c>
       <c r="G3" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="J3" s="2">
+        <v>1477</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>1477</v>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G4" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="J4" s="2">
+        <v>1477</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>1482</v>
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>16</v>
@@ -1098,62 +1136,71 @@
       <c r="H5" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="J5" s="2">
+        <v>1482</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="4">
+        <v>42461</v>
+      </c>
+      <c r="F6" s="4">
+        <v>42461</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="2">
         <v>1748</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="2">
-        <v>2</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>238</v>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E7" s="4">
-        <v>42461</v>
+        <v>42522</v>
       </c>
       <c r="F7" s="4">
-        <v>42461</v>
+        <v>42522</v>
       </c>
       <c r="G7" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="J7" s="2">
+        <v>238</v>
+      </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>238</v>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>24</v>
@@ -1176,123 +1223,138 @@
       <c r="H8" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="J8" s="2">
+        <v>238</v>
+      </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="4">
+        <v>42552</v>
+      </c>
+      <c r="F9" s="4">
+        <v>42552</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="2">
         <v>238</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="4">
-        <v>42522</v>
-      </c>
-      <c r="F9" s="4">
-        <v>42522</v>
-      </c>
-      <c r="G9" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>24</v>
-      </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>265</v>
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G10" s="2">
         <v>1</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>28</v>
+        <v>33</v>
+      </c>
+      <c r="J10" s="2">
+        <v>265</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <v>1501</v>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>32</v>
+      <c r="E11" s="4">
+        <v>42583</v>
+      </c>
+      <c r="F11" s="4">
+        <v>42583</v>
       </c>
       <c r="G11" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
+      </c>
+      <c r="J11" s="2">
+        <v>1501</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
-        <v>1307</v>
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="4">
-        <v>42583</v>
-      </c>
-      <c r="F12" s="4">
-        <v>42583</v>
+      <c r="E12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="G12" s="2">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>33</v>
+        <v>20</v>
+      </c>
+      <c r="J12" s="2">
+        <v>1307</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
-        <v>1307</v>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>19</v>
@@ -1304,63 +1366,76 @@
         <v>1</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>33</v>
+        <v>37</v>
+      </c>
+      <c r="J13" s="2">
+        <v>1307</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
-        <v>1307</v>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="4">
-        <v>42552</v>
-      </c>
-      <c r="F14" s="4">
-        <v>42552</v>
+        <v>22</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="G14" s="2">
         <v>1</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
+      </c>
+      <c r="J14" s="2">
+        <v>1307</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
-        <v>1535</v>
+    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="G15" s="2">
         <v>1</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
+      </c>
+      <c r="J15" s="2">
+        <v>1535</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H15"/>
+  <autoFilter ref="A1:H15">
+    <sortState ref="A2:H15">
+      <sortCondition ref="C1:C15"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changed the data type of start and end date to LocalDate
</commit_message>
<xml_diff>
--- a/ExcelFiles/HRNet.xlsx
+++ b/ExcelFiles/HRNet.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="47">
   <si>
     <t>Worker: Worker ID</t>
   </si>
@@ -1069,11 +1069,11 @@
       <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="4">
-        <v>42398</v>
+      <c r="F3" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="G3" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>8</v>

</xml_diff>